<commit_message>
global menu, shoulder menu を追加
</commit_message>
<xml_diff>
--- a/tests/px2/px-files/sitemaps/sitemap.xlsx
+++ b/tests/px2/px-files/sitemaps/sitemap.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>row_definition=8&amp;row_data_start=9&amp;skip_empty_col=20&amp;version=2.0.9-alpha.1%2Bnb</t>
   </si>
@@ -23,7 +23,7 @@
     <t>「Pickles 2 Practice 1」 サイトマップ</t>
   </si>
   <si>
-    <t>Exported: 2018-03-23 17:07:39</t>
+    <t>Exported: 2018-04-20 20:19:47</t>
   </si>
   <si>
     <t>ページID</t>
@@ -134,6 +134,12 @@
     <t>/</t>
   </si>
   <si>
+    <t>home,sample,pickles2</t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
     <t>Sample 001</t>
   </si>
   <si>
@@ -144,6 +150,18 @@
   </si>
   <si>
     <t>/sample2/</t>
+  </si>
+  <si>
+    <t>HELP 1</t>
+  </si>
+  <si>
+    <t>/help/</t>
+  </si>
+  <si>
+    <t>HELP 2</t>
+  </si>
+  <si>
+    <t>/help/2.html</t>
   </si>
   <si>
     <t>EndOfData</t>
@@ -631,7 +649,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
@@ -828,11 +846,17 @@
         <v>38</v>
       </c>
       <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
+      <c r="P9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
@@ -842,7 +866,7 @@
       <c r="A10" s="4"/>
       <c r="B10" s="6"/>
       <c r="C10" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -852,15 +876,19 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
-      <c r="R10" s="4"/>
+      <c r="R10" s="4">
+        <v>1</v>
+      </c>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
@@ -869,7 +897,7 @@
       <c r="A11" s="4"/>
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -879,43 +907,105 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
+      <c r="M11" s="4">
+        <v>1</v>
+      </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
-      <c r="R11" s="4"/>
+      <c r="R11" s="4">
+        <v>1</v>
+      </c>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
     </row>
-    <row r="14" spans="1:21" customHeight="1" ht="5">
-      <c r="A14" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
+    <row r="12" spans="1:21">
+      <c r="A12" s="4"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="4"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+    </row>
+    <row r="16" spans="1:21" customHeight="1" ht="5">
+      <c r="A16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>